<commit_message>
update db:add primary key to tables
</commit_message>
<xml_diff>
--- a/teamcoop/db/dev/表结构设计.xlsx
+++ b/teamcoop/db/dev/表结构设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="856" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="856" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -767,15 +767,16 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -790,28 +791,37 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -911,10 +921,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -926,30 +936,38 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1025,7 +1043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1111,7 +1129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update db:add cloumn level to table user
</commit_message>
<xml_diff>
--- a/teamcoop/db/dev/表结构设计.xlsx
+++ b/teamcoop/db/dev/表结构设计.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="856" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="856"/>
   </bookViews>
   <sheets>
     <sheet name="user" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -284,6 +284,14 @@
   </si>
   <si>
     <t>任务评论表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1：管理员 2：普通用户</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -633,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -672,49 +680,57 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1043,7 +1059,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>